<commit_message>
tidying and summarizzation of VMH / ARC smfish cell phenotypes (gene+/-, gene +/-, ...) by sex
</commit_message>
<xml_diff>
--- a/NPY-NR5A1-CRHR2-CYP26A1 smFISH HALO Outputs/Results/HYP_ARC_Selected.xlsx
+++ b/NPY-NR5A1-CRHR2-CYP26A1 smFISH HALO Outputs/Results/HYP_ARC_Selected.xlsx
@@ -1,21 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmulvey/Desktop/KM Lab/local_hthspatial/NPY-NR5A1-CRHR2-CYP26A1 smFISH HALO Outputs/Results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7868018A-AAEC-1A43-9625-378954A7D327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>Br1735_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br6588_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br5993_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br6197_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br5459_VMH_ARC</t>
+  </si>
+  <si>
+    <t>520+570+620-690+</t>
+  </si>
+  <si>
+    <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
+  </si>
+  <si>
+    <t>520+570+620-690-</t>
+  </si>
+  <si>
+    <t>520+570-620+690+</t>
+  </si>
+  <si>
+    <t>520+570-620-690+</t>
+  </si>
+  <si>
+    <t>520+570-620-690-</t>
+  </si>
+  <si>
+    <t>520-570+620+690+</t>
+  </si>
+  <si>
+    <t>520-570+620+690-</t>
+  </si>
+  <si>
+    <t>520-570+620-690+</t>
+  </si>
+  <si>
+    <t>520-570+620-690-</t>
+  </si>
+  <si>
+    <t>520-570-620+690+</t>
+  </si>
+  <si>
+    <t>520-570-620+690-</t>
+  </si>
+  <si>
+    <t>520-570-620-690+</t>
+  </si>
+  <si>
+    <t>520-570-620-690-</t>
+  </si>
+  <si>
+    <t>Br8667_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br1225_VMH_ARC</t>
+  </si>
+  <si>
+    <t>Br8741_VMH_ARC</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +146,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +198,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +267,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,75 +443,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>phenotype</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>file_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Br1223_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Br1735_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Br6588_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Br5993_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Br6197_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Br5459_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Br8471_VMH_ARC</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>VMH_ARC</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>520+570+620-690+</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -445,16 +520,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>520+570+620-690-</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -481,16 +552,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>520+570-620+690+</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -517,16 +584,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>520+570-620-690+</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5">
         <v>54</v>
@@ -553,16 +616,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>520+570-620-690-</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
       <c r="C6">
         <v>234</v>
@@ -589,16 +648,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>520-570+620+690+</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -625,16 +680,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>520-570+620+690-</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>48</v>
@@ -661,16 +712,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>520-570+620-690+</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>28</v>
@@ -697,16 +744,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>520-570+620-690-</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
       </c>
       <c r="C10">
         <v>75</v>
@@ -733,16 +776,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>520-570-620+690+</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -769,16 +808,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>520-570-620+690-</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -805,16 +840,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>520-570-620-690+</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
       </c>
       <c r="C13">
         <v>584</v>
@@ -841,16 +872,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>520-570-620-690-</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>HYP - ARC Selected 2 NPY CRHR2 NR5A1 CYP26A1 selected.xlsx</t>
-        </is>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
       </c>
       <c r="C14">
         <v>4630</v>

</xml_diff>